<commit_message>
added analysis by cell
</commit_message>
<xml_diff>
--- a/PFF_HTRA1/Analysis_1_103124.xlsx
+++ b/PFF_HTRA1/Analysis_1_103124.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>48</v>
@@ -476,10 +476,10 @@
         <v>34025</v>
       </c>
       <c r="E2" t="n">
-        <v>924</v>
+        <v>1145</v>
       </c>
       <c r="F2" t="n">
-        <v>272</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3">
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>163</v>
       </c>
       <c r="C3" t="n">
         <v>13</v>
@@ -498,10 +498,10 @@
         <v>33151</v>
       </c>
       <c r="E3" t="n">
-        <v>765</v>
+        <v>8507</v>
       </c>
       <c r="F3" t="n">
-        <v>98</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C4" t="n">
         <v>13</v>
@@ -520,10 +520,10 @@
         <v>33370</v>
       </c>
       <c r="E4" t="n">
-        <v>2111</v>
+        <v>3031</v>
       </c>
       <c r="F4" t="n">
-        <v>114</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>22</v>
@@ -542,7 +542,7 @@
         <v>37943</v>
       </c>
       <c r="E5" t="n">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -564,7 +564,7 @@
         <v>29167</v>
       </c>
       <c r="E6" t="n">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>20</v>
@@ -586,7 +586,7 @@
         <v>35523</v>
       </c>
       <c r="E7" t="n">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -599,7 +599,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>21</v>
@@ -608,10 +608,10 @@
         <v>48918</v>
       </c>
       <c r="E8" t="n">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -630,7 +630,7 @@
         <v>45917</v>
       </c>
       <c r="E9" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
         <v>29</v>
@@ -652,7 +652,7 @@
         <v>48231</v>
       </c>
       <c r="E10" t="n">
-        <v>1388</v>
+        <v>881</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -665,7 +665,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
         <v>30</v>
@@ -674,10 +674,10 @@
         <v>49050</v>
       </c>
       <c r="E11" t="n">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="F11" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
         <v>26</v>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>766</v>
+        <v>887</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>332</v>
+        <v>275</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14" t="n">
         <v>24</v>
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>220</v>
+        <v>334</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C19" t="n">
         <v>23</v>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>972</v>
+        <v>12040</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
         <v>21</v>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C22" t="n">
         <v>28</v>
@@ -916,10 +916,10 @@
         <v>29213</v>
       </c>
       <c r="E22" t="n">
-        <v>2612</v>
+        <v>1921</v>
       </c>
       <c r="F22" t="n">
-        <v>808</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23">
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
         <v>27</v>
@@ -938,10 +938,10 @@
         <v>22796</v>
       </c>
       <c r="E23" t="n">
-        <v>842</v>
+        <v>1034</v>
       </c>
       <c r="F23" t="n">
-        <v>97</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
         <v>35</v>
@@ -960,10 +960,10 @@
         <v>29868</v>
       </c>
       <c r="E24" t="n">
-        <v>447</v>
+        <v>315</v>
       </c>
       <c r="F24" t="n">
-        <v>328</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25">
@@ -973,7 +973,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C25" t="n">
         <v>37</v>
@@ -982,10 +982,10 @@
         <v>32997</v>
       </c>
       <c r="E25" t="n">
-        <v>3129</v>
+        <v>29853</v>
       </c>
       <c r="F25" t="n">
-        <v>277</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26">
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C26" t="n">
         <v>24</v>
@@ -1004,10 +1004,10 @@
         <v>19241</v>
       </c>
       <c r="E26" t="n">
-        <v>1492</v>
+        <v>2652</v>
       </c>
       <c r="F26" t="n">
-        <v>422</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
         <v>18</v>
@@ -1026,7 +1026,7 @@
         <v>27158</v>
       </c>
       <c r="E27" t="n">
-        <v>563</v>
+        <v>67</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C28" t="n">
         <v>40</v>
@@ -1048,10 +1048,10 @@
         <v>18244</v>
       </c>
       <c r="E28" t="n">
-        <v>1473</v>
+        <v>414</v>
       </c>
       <c r="F28" t="n">
-        <v>93</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29">
@@ -1061,7 +1061,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="n">
         <v>39</v>
@@ -1070,7 +1070,7 @@
         <v>30255</v>
       </c>
       <c r="E29" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1092,7 +1092,7 @@
         <v>18871</v>
       </c>
       <c r="E30" t="n">
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C31" t="n">
         <v>30</v>
@@ -1114,10 +1114,10 @@
         <v>35519</v>
       </c>
       <c r="E31" t="n">
-        <v>950</v>
+        <v>3324</v>
       </c>
       <c r="F31" t="n">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -1136,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>409</v>
+        <v>428</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" t="n">
         <v>19</v>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>214</v>
+        <v>336</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C34" t="n">
         <v>16</v>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>735</v>
+        <v>1029</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1202,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>676</v>
+        <v>817</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1215,7 +1215,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C36" t="n">
         <v>26</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>23641</v>
+        <v>25688</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>1630</v>
+        <v>1776</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C38" t="n">
         <v>27</v>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>1906</v>
+        <v>2349</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1281,7 +1281,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C39" t="n">
         <v>30</v>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>862</v>
+        <v>1109</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C40" t="n">
         <v>44</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>2001</v>
+        <v>9867</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>713</v>
+        <v>759</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>

</xml_diff>